<commit_message>
Uploading TEP buildings data files
</commit_message>
<xml_diff>
--- a/InputData/bldgs/EoDSDwSP/Elasticity of Dist Solar Deployment wrt Subsidy Perc.xlsx
+++ b/InputData/bldgs/EoDSDwSP/Elasticity of Dist Solar Deployment wrt Subsidy Perc.xlsx
@@ -1,71 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\EoDSDwSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tepenergy394-my.sharepoint.com/personal/onedrive_tep-energy_ch/Documents/TEP/_projects/1509_Agora_EPS/working/EPS Modelling_TEP_result/bldgs/EoDSDwSP/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_BA10A606E3B3ABE6F7014F81ED4C65C70EC4A7B8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56DB95E0-6B83-47B4-ABFB-FD2FE611855E}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12090"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Calculations" sheetId="3" r:id="rId2"/>
     <sheet name="EoDSDwSP" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
+    <t>EoDSDwSP Elasticity of Distributed Solar Deployment wrt Subsidy Perc</t>
+  </si>
+  <si>
     <t>Source:</t>
   </si>
   <si>
+    <t>Bloomberg New Energy Finance</t>
+  </si>
+  <si>
+    <t>How extending the investment tax credit would affect US solar build</t>
+  </si>
+  <si>
+    <t>http://www.seia.org/sites/default/files/resources/BNEF_SEIA%20Solar%20Forecast_15%20September%202015.pdf</t>
+  </si>
+  <si>
+    <t>Page 3 ("Residential") and Page 4 ("Commercial and Industrial")</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Elasticities intended to reflect change in deployment with changing</t>
+  </si>
+  <si>
+    <t>distributed solar price (through subsidies).</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>BAU Deployment 2015-2022 (GW)</t>
+  </si>
+  <si>
+    <t>Deployment with Extended ITC 2015-2022 (GW)</t>
+  </si>
+  <si>
+    <t>% Increase due to ITC</t>
+  </si>
+  <si>
     <t>Residential</t>
   </si>
   <si>
     <t>Commercial</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>ITC Incentive Level</t>
   </si>
   <si>
+    <t>of system cost</t>
+  </si>
+  <si>
     <t>Elasticity of Distributed Solar Deployment with respect to ITC Incentive Level</t>
   </si>
   <si>
-    <t>Bloomberg New Energy Finance</t>
-  </si>
-  <si>
-    <t>How extending the investment tax credit would affect US solar build</t>
-  </si>
-  <si>
-    <t>http://www.seia.org/sites/default/files/resources/BNEF_SEIA%20Solar%20Forecast_15%20September%202015.pdf</t>
-  </si>
-  <si>
-    <t>Page 3 ("Residential") and Page 4 ("Commercial and Industrial")</t>
-  </si>
-  <si>
-    <t>EoDSDwSP Elasticity of Distributed Solar Deployment wrt Subsidy Perc</t>
-  </si>
-  <si>
-    <t>of system cost</t>
-  </si>
-  <si>
-    <t>% Increase due to ITC</t>
-  </si>
-  <si>
-    <t>BAU Deployment 2015-2022 (GW)</t>
-  </si>
-  <si>
-    <t>Deployment with Extended ITC 2015-2022 (GW)</t>
+    <t>Elasticity (dimensionless)</t>
   </si>
   <si>
     <t>Urban Residential</t>
@@ -73,23 +102,11 @@
   <si>
     <t>Rural Residential</t>
   </si>
-  <si>
-    <t>Notes:</t>
-  </si>
-  <si>
-    <t>Elasticities intended to reflect change in deployment with changing</t>
-  </si>
-  <si>
-    <t>distributed solar price (through subsidies).</t>
-  </si>
-  <si>
-    <t>Elasticity (dimensionless)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -169,9 +186,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -209,9 +226,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,7 +263,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,7 +298,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -454,61 +471,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -518,36 +535,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>15.7</v>
@@ -560,9 +579,9 @@
         <v>0.43949044585987279</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>12.9</v>
@@ -575,36 +594,36 @@
         <v>0.37984496124031009</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>0.3</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B9" s="6">
         <f>D2/$A$6</f>
         <v>1.4649681528662426</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B10" s="6">
         <f>D3/$A$6</f>
@@ -618,7 +637,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -628,37 +647,37 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6">
         <f>Calculations!B9</f>
         <v>1.4649681528662426</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6">
         <f>B2</f>
         <v>1.4649681528662426</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6">
         <f>Calculations!B10</f>
@@ -668,4 +687,270 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ecf9d80fe0681d8e397c19ef62846c2e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="928f64266605fa42fea75ae7d7349071" ns2:_="" ns3:_="">
+    <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <xsd:import namespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="00484652-42e1-479e-92f4-fb0efddcdf60" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildmarkierungen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="eca5b831-c3dc-41cf-bd85-218b82cecb21" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c5b79d03-3bfd-4c46-9947-056a2403f6c9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Freigegeben für" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Freigegeben für - Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD4D7D1B-7C9E-49B8-90E5-FC6880DF8B13}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D54B60E-2F86-4D5A-99F9-98D0789D2616}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25E603D1-B9EE-4BE6-8501-7C23E35D6F39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>